<commit_message>
Added parser script, parsetable fixes, and scanner bug fixes
</commit_message>
<xml_diff>
--- a/doc/parsetable.xlsx
+++ b/doc/parsetable.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/571e7dd58f640a97/Documents/Python/Klein-compiler/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C87B416C-A24A-48CD-85E0-E8DF6B5BB70C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{C87B416C-A24A-48CD-85E0-E8DF6B5BB70C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9DCF06A6-F1FE-46DA-8A47-C63BFC60A931}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3D7752D6-DD4A-4D5B-B337-391F676AF2DB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3D7752D6-DD4A-4D5B-B337-391F676AF2DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -196,15 +196,6 @@
     <t>exp := simexp exp'</t>
   </si>
   <si>
-    <t>exp' := = simexp</t>
-  </si>
-  <si>
-    <t>exp' := &lt; simexp</t>
-  </si>
-  <si>
-    <t>simexp := term simexp'</t>
-  </si>
-  <si>
     <t>simexp' := ε</t>
   </si>
   <si>
@@ -277,9 +268,6 @@
     <t>FA' := ε</t>
   </si>
   <si>
-    <t>FA" := , FA</t>
-  </si>
-  <si>
     <t xml:space="preserve">literal := int-lit </t>
   </si>
   <si>
@@ -310,10 +298,22 @@
     <t>parmlist := FP</t>
   </si>
   <si>
-    <t>exp'  := ε</t>
-  </si>
-  <si>
     <t>body := exp</t>
+  </si>
+  <si>
+    <t>FA' := , FA</t>
+  </si>
+  <si>
+    <t>exp'  :=  ε</t>
+  </si>
+  <si>
+    <t>exp'  := &lt;  simexp</t>
+  </si>
+  <si>
+    <t>simexp :=  term simexp'</t>
+  </si>
+  <si>
+    <t>exp'  := = simexp</t>
   </si>
 </sst>
 </file>
@@ -702,15 +702,15 @@
   <dimension ref="A1:Y69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.140625" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -787,7 +787,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -820,7 +820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -853,7 +853,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -884,7 +884,7 @@
       <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -917,7 +917,7 @@
       <c r="X5" s="1"/>
       <c r="Y5" s="1"/>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -948,7 +948,7 @@
       <c r="X6" s="1"/>
       <c r="Y6" s="1"/>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -981,7 +981,7 @@
       </c>
       <c r="Y7" s="1"/>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1012,7 +1012,7 @@
       <c r="X8" s="1"/>
       <c r="Y8" s="1"/>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1045,7 +1045,7 @@
       <c r="X9" s="1"/>
       <c r="Y9" s="1"/>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1090,7 +1090,7 @@
       <c r="X10" s="1"/>
       <c r="Y10" s="1"/>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1121,7 +1121,7 @@
       <c r="X11" s="1"/>
       <c r="Y11" s="1"/>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1164,7 +1164,7 @@
       <c r="X12" s="1"/>
       <c r="Y12" s="1"/>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1209,10 +1209,10 @@
       </c>
       <c r="U13" s="1"/>
       <c r="V13" s="1">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="W13" s="1">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="X13" s="1">
         <v>17</v>
@@ -1221,7 +1221,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1264,7 +1264,7 @@
       <c r="X14" s="1"/>
       <c r="Y14" s="1"/>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1289,17 +1289,17 @@
       </c>
       <c r="M15" s="1"/>
       <c r="N15" s="1">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O15" s="1"/>
       <c r="P15" s="1">
         <v>21</v>
       </c>
       <c r="Q15" s="1">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="R15" s="1">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="S15" s="1">
         <v>21</v>
@@ -1321,7 +1321,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1364,7 +1364,7 @@
       <c r="X16" s="1"/>
       <c r="Y16" s="1"/>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1385,7 +1385,7 @@
         <v>26</v>
       </c>
       <c r="L17" s="1">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="M17" s="1"/>
       <c r="N17" s="1">
@@ -1402,10 +1402,10 @@
         <v>26</v>
       </c>
       <c r="S17" s="1">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="T17" s="1">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="U17" s="1"/>
       <c r="V17" s="1">
@@ -1421,7 +1421,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1464,7 +1464,7 @@
       <c r="X18" s="1"/>
       <c r="Y18" s="1"/>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1523,7 +1523,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1568,7 +1568,7 @@
       <c r="X20" s="1"/>
       <c r="Y20" s="1"/>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1611,7 +1611,7 @@
       <c r="X21" s="1"/>
       <c r="Y21" s="1"/>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1644,7 +1644,7 @@
       </c>
       <c r="Y22" s="1"/>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1677,308 +1677,308 @@
       <c r="X23" s="1"/>
       <c r="Y23" s="1"/>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
     </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
     </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
     </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
     </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
     </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
     </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
     </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
     </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
     </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
     </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
       <c r="F54" s="2"/>
     </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
       <c r="F55" s="2"/>
     </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
     </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
       <c r="F57" s="2"/>
     </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
     </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
       <c r="F59" s="2"/>
     </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
     </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
     </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
     </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
     </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
     </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
     </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
     </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
       <c r="E67" s="2"/>
       <c r="F67" s="2"/>
     </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
       <c r="E68" s="2"/>
       <c r="F68" s="2"/>
     </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
@@ -2041,133 +2041,133 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F3888B8-E4D4-4C85-AFDA-D656C82E62CA}">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B41" sqref="B41:F41"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2179,7 +2179,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2191,7 +2191,7 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2203,7 +2203,7 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2215,19 +2215,19 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2239,7 +2239,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2251,336 +2251,336 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>53</v>
+        <v>92</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>54</v>
+        <v>90</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>55</v>
+        <v>91</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>

</xml_diff>

<commit_message>
Added more test programs, fixed epsilon handling in parser, updated parse table and firstfollowsets
</commit_message>
<xml_diff>
--- a/doc/parsetable.xlsx
+++ b/doc/parsetable.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/571e7dd58f640a97/Documents/Python/Klein-compiler/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{C87B416C-A24A-48CD-85E0-E8DF6B5BB70C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9DCF06A6-F1FE-46DA-8A47-C63BFC60A931}"/>
+  <xr:revisionPtr revIDLastSave="203" documentId="13_ncr:1_{C87B416C-A24A-48CD-85E0-E8DF6B5BB70C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2D940B78-11C3-4F8C-83DC-A0760996098F}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3D7752D6-DD4A-4D5B-B337-391F676AF2DB}"/>
   </bookViews>
@@ -702,7 +702,7 @@
   <dimension ref="A1:Y69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1611,7 +1611,7 @@
       <c r="X21" s="1"/>
       <c r="Y21" s="1"/>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1987,34 +1987,6 @@
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="B44:F44"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="B36:F36"/>
-    <mergeCell ref="B37:F37"/>
-    <mergeCell ref="B40:F40"/>
-    <mergeCell ref="B41:F41"/>
-    <mergeCell ref="B42:F42"/>
-    <mergeCell ref="B43:F43"/>
-    <mergeCell ref="B38:F38"/>
-    <mergeCell ref="B39:F39"/>
-    <mergeCell ref="B55:F55"/>
-    <mergeCell ref="B56:F56"/>
-    <mergeCell ref="B45:F45"/>
-    <mergeCell ref="B46:F46"/>
-    <mergeCell ref="B47:F47"/>
-    <mergeCell ref="B48:F48"/>
-    <mergeCell ref="B67:F67"/>
-    <mergeCell ref="B68:F68"/>
-    <mergeCell ref="B57:F57"/>
-    <mergeCell ref="B58:F58"/>
-    <mergeCell ref="B59:F59"/>
-    <mergeCell ref="B60:F60"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="B30:F30"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="B32:F32"/>
     <mergeCell ref="B33:F33"/>
     <mergeCell ref="B29:F29"/>
     <mergeCell ref="B69:F69"/>
@@ -2031,6 +2003,34 @@
     <mergeCell ref="B52:F52"/>
     <mergeCell ref="B53:F53"/>
     <mergeCell ref="B54:F54"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="B30:F30"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="B67:F67"/>
+    <mergeCell ref="B68:F68"/>
+    <mergeCell ref="B57:F57"/>
+    <mergeCell ref="B58:F58"/>
+    <mergeCell ref="B59:F59"/>
+    <mergeCell ref="B60:F60"/>
+    <mergeCell ref="B55:F55"/>
+    <mergeCell ref="B56:F56"/>
+    <mergeCell ref="B45:F45"/>
+    <mergeCell ref="B46:F46"/>
+    <mergeCell ref="B47:F47"/>
+    <mergeCell ref="B48:F48"/>
+    <mergeCell ref="B44:F44"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="B36:F36"/>
+    <mergeCell ref="B37:F37"/>
+    <mergeCell ref="B40:F40"/>
+    <mergeCell ref="B41:F41"/>
+    <mergeCell ref="B42:F42"/>
+    <mergeCell ref="B43:F43"/>
+    <mergeCell ref="B38:F38"/>
+    <mergeCell ref="B39:F39"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2041,8 +2041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F3888B8-E4D4-4C85-AFDA-D656C82E62CA}">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2589,35 +2589,6 @@
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="B33:F33"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="B36:F36"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="B44:F44"/>
     <mergeCell ref="B45:F45"/>
@@ -2634,6 +2605,35 @@
     <mergeCell ref="B29:F29"/>
     <mergeCell ref="B30:F30"/>
     <mergeCell ref="B31:F31"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="B36:F36"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B12:F12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Parser changes and Refactored Grammar V2
</commit_message>
<xml_diff>
--- a/doc/parsetable.xlsx
+++ b/doc/parsetable.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/571e7dd58f640a97/Documents/Python/Klein-compiler/doc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dylan\OneDrive\Documents\Python\Klein-compiler\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="203" documentId="13_ncr:1_{C87B416C-A24A-48CD-85E0-E8DF6B5BB70C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2D940B78-11C3-4F8C-83DC-A0760996098F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3A91063-29C1-4B3D-AA0A-C1E6D487665E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1872" yWindow="4032" windowWidth="9876" windowHeight="6600" xr2:uid="{3D7752D6-DD4A-4D5B-B337-391F676AF2DB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{3D7752D6-DD4A-4D5B-B337-391F676AF2DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -199,30 +199,12 @@
     <t>simexp' := ε</t>
   </si>
   <si>
-    <t>simexp' := or term</t>
-  </si>
-  <si>
-    <t>simexp' := + term</t>
-  </si>
-  <si>
-    <t>simexp' := - term</t>
-  </si>
-  <si>
     <t>term := factor term'</t>
   </si>
   <si>
     <t>term' := ε</t>
   </si>
   <si>
-    <t>term' := * factor</t>
-  </si>
-  <si>
-    <t>term' := / factor</t>
-  </si>
-  <si>
-    <t>term' := and factor</t>
-  </si>
-  <si>
     <t>factor := literal</t>
   </si>
   <si>
@@ -310,10 +292,28 @@
     <t>exp'  := &lt;  simexp</t>
   </si>
   <si>
-    <t>simexp :=  term simexp'</t>
-  </si>
-  <si>
     <t>exp'  := = simexp</t>
+  </si>
+  <si>
+    <t>simexp' := or term simexp'</t>
+  </si>
+  <si>
+    <t>simexp' := + term simexp'</t>
+  </si>
+  <si>
+    <t>simexp' := - term simexp'</t>
+  </si>
+  <si>
+    <t>term' := * factor term'</t>
+  </si>
+  <si>
+    <t>term' := / factor term'</t>
+  </si>
+  <si>
+    <t>term' := and factor term'</t>
+  </si>
+  <si>
+    <t>simexp :=  term</t>
   </si>
 </sst>
 </file>
@@ -376,10 +376,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -701,8 +697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4E9D6FE-A75B-4074-88DB-FFFA902B6AFB}">
   <dimension ref="A1:Y69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1987,34 +1983,6 @@
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="B44:F44"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="B36:F36"/>
-    <mergeCell ref="B37:F37"/>
-    <mergeCell ref="B40:F40"/>
-    <mergeCell ref="B41:F41"/>
-    <mergeCell ref="B42:F42"/>
-    <mergeCell ref="B43:F43"/>
-    <mergeCell ref="B38:F38"/>
-    <mergeCell ref="B39:F39"/>
-    <mergeCell ref="B55:F55"/>
-    <mergeCell ref="B56:F56"/>
-    <mergeCell ref="B45:F45"/>
-    <mergeCell ref="B46:F46"/>
-    <mergeCell ref="B47:F47"/>
-    <mergeCell ref="B48:F48"/>
-    <mergeCell ref="B67:F67"/>
-    <mergeCell ref="B68:F68"/>
-    <mergeCell ref="B57:F57"/>
-    <mergeCell ref="B58:F58"/>
-    <mergeCell ref="B59:F59"/>
-    <mergeCell ref="B60:F60"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="B30:F30"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="B32:F32"/>
     <mergeCell ref="B33:F33"/>
     <mergeCell ref="B29:F29"/>
     <mergeCell ref="B69:F69"/>
@@ -2031,6 +1999,34 @@
     <mergeCell ref="B52:F52"/>
     <mergeCell ref="B53:F53"/>
     <mergeCell ref="B54:F54"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="B30:F30"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="B67:F67"/>
+    <mergeCell ref="B68:F68"/>
+    <mergeCell ref="B57:F57"/>
+    <mergeCell ref="B58:F58"/>
+    <mergeCell ref="B59:F59"/>
+    <mergeCell ref="B60:F60"/>
+    <mergeCell ref="B55:F55"/>
+    <mergeCell ref="B56:F56"/>
+    <mergeCell ref="B45:F45"/>
+    <mergeCell ref="B46:F46"/>
+    <mergeCell ref="B47:F47"/>
+    <mergeCell ref="B48:F48"/>
+    <mergeCell ref="B44:F44"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="B36:F36"/>
+    <mergeCell ref="B37:F37"/>
+    <mergeCell ref="B40:F40"/>
+    <mergeCell ref="B41:F41"/>
+    <mergeCell ref="B42:F42"/>
+    <mergeCell ref="B43:F43"/>
+    <mergeCell ref="B38:F38"/>
+    <mergeCell ref="B39:F39"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2041,18 +2037,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F3888B8-E4D4-4C85-AFDA-D656C82E62CA}">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:F4"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
@@ -2064,7 +2060,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -2076,7 +2072,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -2088,7 +2084,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -2100,7 +2096,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -2112,7 +2108,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -2124,7 +2120,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -2136,7 +2132,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -2148,7 +2144,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -2160,7 +2156,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -2220,7 +2216,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -2256,7 +2252,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -2268,7 +2264,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -2280,7 +2276,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -2292,7 +2288,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -2316,7 +2312,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>54</v>
+        <v>86</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -2328,7 +2324,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>55</v>
+        <v>87</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -2340,7 +2336,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>56</v>
+        <v>88</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -2352,7 +2348,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -2364,7 +2360,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -2376,7 +2372,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -2388,7 +2384,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -2400,7 +2396,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>61</v>
+        <v>91</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
@@ -2412,7 +2408,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -2424,7 +2420,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -2436,7 +2432,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
@@ -2448,7 +2444,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
@@ -2460,7 +2456,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -2472,7 +2468,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -2484,7 +2480,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
@@ -2496,7 +2492,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
@@ -2508,7 +2504,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
@@ -2520,7 +2516,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
@@ -2532,7 +2528,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
@@ -2544,7 +2540,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
@@ -2556,7 +2552,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
@@ -2568,7 +2564,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
@@ -2580,7 +2576,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
@@ -2589,35 +2585,6 @@
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="B33:F33"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="B36:F36"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="B44:F44"/>
     <mergeCell ref="B45:F45"/>
@@ -2634,6 +2601,35 @@
     <mergeCell ref="B29:F29"/>
     <mergeCell ref="B30:F30"/>
     <mergeCell ref="B31:F31"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="B36:F36"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B12:F12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>